<commit_message>
functional reqs - freezed
</commit_message>
<xml_diff>
--- a/docs/kcap-nevar-fun_reqs.xlsx
+++ b/docs/kcap-nevar-fun_reqs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t xml:space="preserve">Req status (*)</t>
   </si>
@@ -49,99 +49,105 @@
     <t xml:space="preserve">Notes, questions</t>
   </si>
   <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTH-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User signup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anonymous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an account, to become a voter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/signup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Mandatory fields: [username, password, email]; 2. check format fields: [email]; 3. Unique fields: [username, email]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAYBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTH-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password is lost: reset it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/passwd_recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. email inserted must be == email set in AUTH-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTH-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log in to application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Mandatory fields: [username, password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTH-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authenticated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log out from application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Session started in AUTH-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLL-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pizza poll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click “I love it button”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/poll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Only auth user can vote.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each vote is registered – it increments a persistent a user_votes_sum</t>
+  </si>
+  <si>
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
-    <t xml:space="preserve">N/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTH-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User signup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anonymous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create an account, to become a voter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/signup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Mandatory fields: [username, password, email]; 2. check format fields: [email]; 3. Unique fields: [username, email]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTH-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password is lost: reset it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/passwd_recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. email inserted must be == email set in AUTH-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTH-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log in to application </t>
-  </si>
-  <si>
-    <t xml:space="preserve">/login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Mandatory fields: [username, password]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTH-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authenticated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log out from application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Session started in AUTH-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLL-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pizza poll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click “I love it button”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/poll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Only auth user can vote.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Before voting, should be choosen a preferred pizza? The “vote” can be submitted w/o choosing a preferred one?</t>
-  </si>
-  <si>
     <t xml:space="preserve">POLL-02</t>
   </si>
   <si>
@@ -154,10 +160,13 @@
     <t xml:space="preserve">View “Top 10 voters” </t>
   </si>
   <si>
-    <t xml:space="preserve">(*): Can be: N/D, WIP, OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doc revision: 20180621_1723</t>
+    <t xml:space="preserve">For each user is showed a bar in a chart with sum of POLL-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(*): Can be: N/D, WIP, OK, MAYBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc revision: 20180622_1523</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +228,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9999FF"/>
+        <bgColor rgb="FFCC99FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -264,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,12 +296,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -346,7 +365,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF99FF99"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF9999"/>
@@ -380,13 +399,13 @@
   </sheetPr>
   <dimension ref="1:23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7857142857143"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6020408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
@@ -434,192 +453,192 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>44</v>
+      <c r="A21" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>